<commit_message>
update Tierra de Osos DB project
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lenovo-my.sharepoint.com/personal/tmarsico_lenovo_com/Documents/Personal/programacion/coderhouse/81860sql/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78071814-3C81-4276-B868-F1D98666EE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{78071814-3C81-4276-B868-F1D98666EE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7886F52A-D6EA-4BC8-A430-7A18758DEDB7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{48623857-4B71-4B27-BD86-D53DB7FA56F6}"/>
   </bookViews>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="67">
   <si>
     <t>Abrev.</t>
   </si>
   <si>
-    <t>id_cliente</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -71,16 +65,178 @@
     <t>VARCHAR(100)</t>
   </si>
   <si>
-    <t>VARCHAR(150)</t>
-  </si>
-  <si>
-    <t>Clave</t>
-  </si>
-  <si>
     <t>PK</t>
   </si>
   <si>
     <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>Clave / Restricciones</t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>SERIAL</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>supplier_id</t>
+  </si>
+  <si>
+    <t>Identificador del proveedor</t>
+  </si>
+  <si>
+    <t>Nombre del proveedor</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>Teléfono</t>
+  </si>
+  <si>
+    <t>VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>CUSTOMERS</t>
+  </si>
+  <si>
+    <t>SUPPLIERS</t>
+  </si>
+  <si>
+    <t>CATEGORIES</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>Identificador de categoría</t>
+  </si>
+  <si>
+    <t>Nombre de la categoría</t>
+  </si>
+  <si>
+    <t>PRODUCTS</t>
+  </si>
+  <si>
+    <t>product_id</t>
+  </si>
+  <si>
+    <t>Identificador del producto</t>
+  </si>
+  <si>
+    <t>Nombre del producto</t>
+  </si>
+  <si>
+    <t>Categoría</t>
+  </si>
+  <si>
+    <t>FK REFERENCES categories(category_id)</t>
+  </si>
+  <si>
+    <t>Proveedor</t>
+  </si>
+  <si>
+    <t>FK REFERENCES suppliers(supplier_id)</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>DECIMAL(10,2)</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>Stock disponible</t>
+  </si>
+  <si>
+    <t>DEFAULT 0</t>
+  </si>
+  <si>
+    <t>ORDERS</t>
+  </si>
+  <si>
+    <t>order_id</t>
+  </si>
+  <si>
+    <t>Identificador de orden</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>FK REFERENCES customers(customer_id)</t>
+  </si>
+  <si>
+    <t>order_date</t>
+  </si>
+  <si>
+    <t>Fecha de orden</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>DEFAULT CURRENT_DATE</t>
+  </si>
+  <si>
+    <t>total_amount</t>
+  </si>
+  <si>
+    <t>Total del pedido</t>
+  </si>
+  <si>
+    <t>ORDER_ITEMS</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Identificador del ítem</t>
+  </si>
+  <si>
+    <t>Orden</t>
+  </si>
+  <si>
+    <t>FK REFERENCES orders(order_id)</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>FK REFERENCES products(product_id)</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>unit_price</t>
+  </si>
+  <si>
+    <t>Precio unitario</t>
   </si>
 </sst>
 </file>
@@ -136,13 +292,78 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AD8B4356-F771-43B4-8BC3-11EF8DA61FA4}" name="Table2" displayName="Table2" ref="A1:D4" totalsRowShown="0">
-  <autoFilter ref="A1:D4" xr:uid="{AD8B4356-F771-43B4-8BC3-11EF8DA61FA4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AD8B4356-F771-43B4-8BC3-11EF8DA61FA4}" name="Table2" displayName="Table2" ref="A2:D5" totalsRowShown="0">
+  <autoFilter ref="A2:D5" xr:uid="{AD8B4356-F771-43B4-8BC3-11EF8DA61FA4}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{8F655E56-F1F3-4078-A71F-00F08C8B52A1}" name="Abrev."/>
     <tableColumn id="2" xr3:uid="{8B28328E-4E5E-4EA5-8BDD-0FEED8537F31}" name="Nombre completo"/>
     <tableColumn id="3" xr3:uid="{1748FA62-0BDC-4817-931A-11262D4027FD}" name="Tipo de dato"/>
-    <tableColumn id="4" xr3:uid="{C0C54D38-A9FC-4DB6-A41B-358340967116}" name="Clave"/>
+    <tableColumn id="4" xr3:uid="{C0C54D38-A9FC-4DB6-A41B-358340967116}" name="Clave / Restricciones"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{650F3CF6-C549-41D4-A3DB-5DF3F593D049}" name="Table3" displayName="Table3" ref="F2:I7" totalsRowShown="0">
+  <autoFilter ref="F2:I7" xr:uid="{650F3CF6-C549-41D4-A3DB-5DF3F593D049}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C1695F63-22DF-4B78-A3C3-7CEBE61F0137}" name="Abrev."/>
+    <tableColumn id="2" xr3:uid="{D2C6F556-EE9B-4CE7-AD1E-023505AE5956}" name="Nombre completo"/>
+    <tableColumn id="3" xr3:uid="{6991348D-BD6D-421C-85A2-1E69D2D1F6A6}" name="Tipo de dato"/>
+    <tableColumn id="4" xr3:uid="{CE1AA4E6-18DA-4C88-B5C3-5BBCDF088FAA}" name="Clave / Restricciones"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{302269A5-6A94-45C8-A62C-E8B2A7E7DE4C}" name="Table4" displayName="Table4" ref="K2:N4" totalsRowShown="0">
+  <autoFilter ref="K2:N4" xr:uid="{302269A5-6A94-45C8-A62C-E8B2A7E7DE4C}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{8CE98188-201F-42EF-9D53-111FB3703EE4}" name="Abrev."/>
+    <tableColumn id="2" xr3:uid="{31EAFDB0-B172-4F48-9C08-4DAEACAC7B0B}" name="Nombre completo"/>
+    <tableColumn id="3" xr3:uid="{01DCF07A-6C31-4E2F-AB15-F0600840CCB8}" name="Tipo de dato"/>
+    <tableColumn id="4" xr3:uid="{106E08DA-CFD1-4D15-9BA9-E9BBD1C059AF}" name="Clave / Restricciones"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4CE87861-7BE4-4CAF-8F80-99235FB29423}" name="Table5" displayName="Table5" ref="P2:S8" totalsRowShown="0">
+  <autoFilter ref="P2:S8" xr:uid="{4CE87861-7BE4-4CAF-8F80-99235FB29423}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{EA84C36A-ECBC-4B82-A2DC-C267F290F351}" name="Abrev."/>
+    <tableColumn id="2" xr3:uid="{CD92FA3C-8C07-4BCC-8E44-72F3B0593757}" name="Nombre completo"/>
+    <tableColumn id="3" xr3:uid="{AF068F2A-00CA-4F9F-AC24-2B2F9FE57360}" name="Tipo de dato"/>
+    <tableColumn id="4" xr3:uid="{ACACAF13-6ACC-4B71-9970-6417923C8650}" name="Clave / Restricciones"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B2EA9F7B-5593-4204-9BDE-23548D3E7119}" name="Table6" displayName="Table6" ref="U2:X6" totalsRowShown="0">
+  <autoFilter ref="U2:X6" xr:uid="{B2EA9F7B-5593-4204-9BDE-23548D3E7119}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{DE0F9C5E-C14D-4F81-A6A6-FEBF51CBE892}" name="Abrev."/>
+    <tableColumn id="2" xr3:uid="{12DCDB40-0B8D-4ED4-9455-F491FBC307BE}" name="Nombre completo"/>
+    <tableColumn id="3" xr3:uid="{99ECA637-673E-4273-BDCE-361813457C6C}" name="Tipo de dato"/>
+    <tableColumn id="4" xr3:uid="{BF0917CE-9CAC-4E14-9278-A2D88C8FD9E1}" name="Clave / Restricciones"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{62B76747-51C8-4332-A07D-DFB43B4CFECD}" name="Table7" displayName="Table7" ref="Z2:AC7" totalsRowShown="0">
+  <autoFilter ref="Z2:AC7" xr:uid="{62B76747-51C8-4332-A07D-DFB43B4CFECD}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{DE5EAFBF-19B5-4B24-A1AF-7E0D32D5E019}" name="Abrev."/>
+    <tableColumn id="2" xr3:uid="{D4B0F670-BB8B-4D98-A7CD-514B41CAAA1B}" name="Nombre completo"/>
+    <tableColumn id="3" xr3:uid="{A50BAB11-FB2E-49B3-85F6-9486187D7EE7}" name="Tipo de dato"/>
+    <tableColumn id="4" xr3:uid="{04ADC2A3-2574-4DF3-A54C-D02956F72C3C}" name="Clave / Restricciones"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -465,77 +686,440 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA2B9B89-738B-4B5C-AD0E-5363736B657C}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:AC8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D4"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AC21" sqref="AC21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" t="s">
+        <v>6</v>
+      </c>
+      <c r="X2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S3" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W3" t="s">
+        <v>13</v>
+      </c>
+      <c r="X3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U4" t="s">
         <v>12</v>
       </c>
+      <c r="V4" t="s">
+        <v>48</v>
+      </c>
+      <c r="W4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" t="s">
+        <v>7</v>
+      </c>
+      <c r="S5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" t="s">
+        <v>50</v>
+      </c>
+      <c r="V5" t="s">
+        <v>51</v>
+      </c>
+      <c r="W5" t="s">
+        <v>52</v>
+      </c>
+      <c r="X5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>37</v>
+      </c>
+      <c r="R6" t="s">
+        <v>7</v>
+      </c>
+      <c r="S6" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" t="s">
+        <v>54</v>
+      </c>
+      <c r="V6" t="s">
+        <v>55</v>
+      </c>
+      <c r="W6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="P8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
+      <c r="S8" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="6">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>